<commit_message>
adding option to have data in the main_page
</commit_message>
<xml_diff>
--- a/vignettes/data/nhanes_data.xlsx
+++ b/vignettes/data/nhanes_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lclem\OneDrive\Documents\GitHub\plhR\vignettes\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/018fd3f915004678/Documents/GitHub/plhR/vignettes/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63FFCD1-71FB-44B3-A637-834E0E506954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{E63FFCD1-71FB-44B3-A637-834E0E506954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACBEDC0E-E5DF-43E8-8FCB-D0C4724CA636}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="785" activeTab="4" xr2:uid="{B26721C4-B7AF-4AF7-A1C0-7CF04F3F9D6A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="785" activeTab="1" xr2:uid="{B26721C4-B7AF-4AF7-A1C0-7CF04F3F9D6A}"/>
   </bookViews>
   <sheets>
     <sheet name="contents" sheetId="1" r:id="rId1"/>
@@ -179,9 +179,6 @@
     <t>geom_point(aes(x = BPDiaAve, y = BPSysAve, colour = AgeDecade)) + labs(x = "Average Diastolic BP", y = "Average Systolic BP") + theme_minimal()</t>
   </si>
   <si>
-    <t>%&gt;% group_by(AgeDecade) %&gt;% summarise(min(BPDiaAve))</t>
-  </si>
-  <si>
     <t>Diagnostics</t>
   </si>
   <si>
@@ -300,6 +297,9 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>%&gt;% group_by(AgeDecade) %&gt;% summarise(min(BPDiaAve, na.rm = TRUE))</t>
   </si>
 </sst>
 </file>
@@ -401,6 +401,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -764,16 +768,16 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -800,7 +804,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12D8BFF4-592C-4E1D-B797-47F7D8E2FB2B}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -835,7 +841,7 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D2" t="s">
         <v>28</v>
@@ -852,7 +858,7 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D3" t="s">
         <v>28</v>
@@ -877,13 +883,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s">
         <v>28</v>
@@ -891,7 +897,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
@@ -913,12 +919,12 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
@@ -945,10 +951,10 @@
         <v>22</v>
       </c>
       <c r="G1" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -976,7 +982,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
         <v>33</v>
@@ -1076,13 +1082,13 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>79</v>
-      </c>
       <c r="D8" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E8" s="4">
         <v>4</v>
@@ -1091,10 +1097,10 @@
         <v>43</v>
       </c>
       <c r="G8" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1128,24 +1134,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1157,8 +1163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27922189-859D-4D68-B6A1-924FFE4722CC}">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D2:D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1189,10 +1195,10 @@
         <v>13</v>
       </c>
       <c r="G1" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -1203,13 +1209,13 @@
         <v>15</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F2" s="4">
         <v>1</v>
@@ -1223,13 +1229,13 @@
         <v>15</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F3" s="4">
         <v>2</v>
@@ -1243,13 +1249,13 @@
         <v>15</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F4" s="4">
         <v>3</v>
@@ -1260,25 +1266,25 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="F5" s="4">
         <v>4</v>
       </c>
       <c r="G5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -1389,8 +1395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A92F21-F729-4BA7-A15C-64ABBF25F2B5}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L1:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1411,7 +1417,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>20</v>
@@ -1446,13 +1452,13 @@
         <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="E2" t="s">
         <v>44</v>
       </c>
       <c r="F2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G2" t="s">
         <v>2</v>
@@ -1461,7 +1467,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1474,7 +1480,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1497,15 +1503,15 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" t="s">
         <v>70</v>
-      </c>
-      <c r="B2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
         <v>26</v>
@@ -1513,15 +1519,15 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
         <v>57</v>
-      </c>
-      <c r="C4" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
         <v>34</v>
@@ -1532,10 +1538,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" t="s">
         <v>59</v>
-      </c>
-      <c r="B6" t="s">
-        <v>60</v>
       </c>
       <c r="C6" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
update to shiny vignette following additions
</commit_message>
<xml_diff>
--- a/vignettes/data/nhanes_data.xlsx
+++ b/vignettes/data/nhanes_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/018fd3f915004678/Documents/GitHub/plhR/vignettes/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{E63FFCD1-71FB-44B3-A637-834E0E506954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACBEDC0E-E5DF-43E8-8FCB-D0C4724CA636}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="14_{B428EE3B-C5F1-4498-98CC-7EDDDE53D703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{864A7BA6-ADB1-49C9-8639-9DFD43242D27}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="785" activeTab="1" xr2:uid="{B26721C4-B7AF-4AF7-A1C0-7CF04F3F9D6A}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="88">
   <si>
     <t>name</t>
   </si>
@@ -300,6 +300,12 @@
   </si>
   <si>
     <t>%&gt;% group_by(AgeDecade) %&gt;% summarise(min(BPDiaAve, na.rm = TRUE))</t>
+  </si>
+  <si>
+    <t>text = "Total individuals in the study", colour = "aqua", icon = "tick"</t>
+  </si>
+  <si>
+    <t>value_box_rows</t>
   </si>
 </sst>
 </file>
@@ -802,10 +808,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12D8BFF4-592C-4E1D-B797-47F7D8E2FB2B}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -814,6 +820,7 @@
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="68.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -838,16 +845,10 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -858,13 +859,13 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
         <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -872,40 +873,57 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
       </c>
       <c r="C6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
         <v>35</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
temp fix in plotly boxplot code as recorded in issue https://github.com/plotly/plotly.R/issues/2032
</commit_message>
<xml_diff>
--- a/vignettes/data/nhanes_data.xlsx
+++ b/vignettes/data/nhanes_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/018fd3f915004678/Documents/GitHub/plhR/vignettes/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="14_{B428EE3B-C5F1-4498-98CC-7EDDDE53D703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{864A7BA6-ADB1-49C9-8639-9DFD43242D27}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="14_{B428EE3B-C5F1-4498-98CC-7EDDDE53D703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47325129-413D-43BB-B896-910CA145FA7F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="785" activeTab="1" xr2:uid="{B26721C4-B7AF-4AF7-A1C0-7CF04F3F9D6A}"/>
+    <workbookView xWindow="10720" yWindow="0" windowWidth="8570" windowHeight="11370" tabRatio="785" firstSheet="5" activeTab="6" xr2:uid="{B26721C4-B7AF-4AF7-A1C0-7CF04F3F9D6A}"/>
   </bookViews>
   <sheets>
     <sheet name="contents" sheetId="1" r:id="rId1"/>
@@ -732,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F49BA2F9-BCCB-4D9C-9237-2952836443FB}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView zoomScale="113" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+    <sheetView topLeftCell="C1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -810,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12D8BFF4-592C-4E1D-B797-47F7D8E2FB2B}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -937,7 +937,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1131,7 +1131,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1182,7 +1182,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1413,8 +1413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A92F21-F729-4BA7-A15C-64ABBF25F2B5}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L1:L5"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1497,8 +1497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE16F053-17FC-4213-9D26-23BD0D46E28F}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>